<commit_message>
create new module on base def excel(fix)
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,6 +470,41 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sss4</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>sss4</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>sss5</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>sss6</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>sss8</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>sss10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
prepare to create modules
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,6 +505,41 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
create modules gui and database
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,6 +540,41 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ddss</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ddss</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ddss</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ddss</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>ddss</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ddss</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
create module deleteiftime those delete userdata if dat exists 3 years old.
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,6 +575,41 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>sss</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
functions dataupdate, getentrytwo and reg convert to modules dataupdate, getuserdata, registration (respectively)
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ssss</t>
+          <t>ss2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -607,6 +607,76 @@
       <c r="G5" t="inlineStr">
         <is>
           <t>ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>ssss</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>228</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>228</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>228</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>228</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>228</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>228</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
rename some function and add excel into registration.py and data_update.py
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -680,6 +680,41 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ss88</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ss88</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ss88</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ss88ss88</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ss88</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>ss88</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>